<commit_message>
update with final participants
</commit_message>
<xml_diff>
--- a/data/Participants.xlsx
+++ b/data/Participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\Zstring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CA2995-2365-4AB3-B039-BD985E17A7C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6395A365-0B5A-453E-8FD1-A05998E2E654}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2625" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -41,12 +41,27 @@
   <si>
     <t>Male</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>glasses</t>
+  </si>
+  <si>
+    <t>left eye tracked</t>
+  </si>
+  <si>
+    <t>Contact lenses</t>
+  </si>
+  <si>
+    <t>glasses; left eye tracked</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,13 +69,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,9 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -362,27 +394,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -393,7 +430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -403,8 +440,11 @@
       <c r="C3" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -415,7 +455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -426,7 +466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -437,7 +477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -448,7 +488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -459,7 +499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -470,7 +510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -481,7 +521,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -492,7 +532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -503,7 +543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -513,8 +553,11 @@
       <c r="C13" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -525,7 +568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -536,7 +579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -547,7 +590,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -557,8 +600,11 @@
       <c r="C17" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -569,7 +615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -580,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -591,7 +637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -602,7 +648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -613,7 +659,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -624,7 +670,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -635,7 +681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -646,7 +692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -657,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -668,7 +714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -678,8 +724,11 @@
       <c r="C28" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -690,7 +739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -701,7 +750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -711,8 +760,11 @@
       <c r="C31" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -722,8 +774,11 @@
       <c r="C32" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -734,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -744,8 +799,11 @@
       <c r="C34" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -755,8 +813,11 @@
       <c r="C35" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -767,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -778,7 +839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -789,7 +850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -799,8 +860,11 @@
       <c r="C39" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -811,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -822,7 +886,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -833,7 +897,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -844,7 +908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -855,7 +919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -866,7 +930,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -877,7 +941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -888,7 +952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -899,7 +963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -910,7 +974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -921,7 +985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -932,7 +996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -943,7 +1007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -954,7 +1018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -965,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -976,7 +1040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -987,7 +1051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -998,7 +1062,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1009,7 +1073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -1020,7 +1084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -1031,7 +1095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -1041,8 +1105,11 @@
       <c r="C61" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -1053,7 +1120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -1061,10 +1128,13 @@
         <v>3</v>
       </c>
       <c r="C63" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1075,7 +1145,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -1086,7 +1156,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -1097,7 +1167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -1108,7 +1178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -1119,7 +1189,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -1129,25 +1199,52 @@
       <c r="C69" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>